<commit_message>
schedule type and bulk upload template
</commit_message>
<xml_diff>
--- a/documents/templates/bulk-upload/12-BulkUploadLocation.xlsx
+++ b/documents/templates/bulk-upload/12-BulkUploadLocation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineshgajjar/Documents/Work/GitLab/YHWorks/Briot/clients/TMML/server/documents/templates/bulk-upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA599B13-8CB4-CF4C-BA49-ED2F1C1C2785}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A6871C-B3F9-A342-BF42-57F0C2890D73}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="16040" xr2:uid="{BDF805E5-0C49-044A-9E09-D74DAAF0D499}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -51,13 +51,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF333333"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -72,8 +85,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,19 +407,19 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="48.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="28" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>